<commit_message>
Version 7 - door sensor tested
</commit_message>
<xml_diff>
--- a/battery_calculations.xlsx
+++ b/battery_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anunez/code-home/platformio-projects/SoilLoraSensor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B785B2A-AEBE-9941-9EB3-69DEF3B10CDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281172F0-AF69-2C49-ABAC-17A5ABEE6116}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="2560" windowWidth="27240" windowHeight="16440" xr2:uid="{274C38AF-7C22-4540-ABA6-4F5A66EA3CC3}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -739,7 +739,7 @@
         <v>2E-3</v>
       </c>
       <c r="H9">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -809,7 +809,7 @@
         <v>1400</v>
       </c>
       <c r="H12">
-        <v>300</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -929,7 +929,7 @@
       </c>
       <c r="H19">
         <f t="shared" ref="H19" si="5">H9*1000</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -962,7 +962,7 @@
       </c>
       <c r="H20">
         <f t="shared" si="6"/>
-        <v>7.0967741935483886E-2</v>
+        <v>4.8458149779735692E-2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -995,7 +995,7 @@
       </c>
       <c r="H23">
         <f>24*365*(H16+H17+H18+H19)/1000</f>
-        <v>18.887533333333334</v>
+        <v>27.647533333333332</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="H24" s="1">
         <f t="shared" si="7"/>
-        <v>15.883492815366749</v>
+        <v>50.637428776045127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>